<commit_message>
TAT Completed Report Modified. 2018/06/28
</commit_message>
<xml_diff>
--- a/Reports/Demo_rep_Report_Iteration_12.xlsx
+++ b/Reports/Demo_rep_Report_Iteration_12.xlsx
@@ -2427,7 +2427,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="67">
+  <fills count="65">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2795,12 +2795,6 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="18"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="none">
         <fgColor indexed="10"/>
       </patternFill>
@@ -2813,12 +2807,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="42"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="23"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4102,7 +4090,7 @@
     <xf applyAlignment="1" applyBorder="1" borderId="10" fillId="52" fontId="40" numFmtId="0" xfId="43">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="10" fillId="62" fontId="43" numFmtId="0" xfId="47" applyFill="true">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="10" fillId="64" fontId="43" numFmtId="0" xfId="47" applyFill="true">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" applyBorder="1" borderId="10" fillId="46" fontId="20" numFmtId="0" xfId="48">
@@ -4285,73 +4273,73 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="64" borderId="0" xfId="0" applyFill="true">
+    <xf numFmtId="0" fontId="0" fillId="63" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">

</xml_diff>